<commit_message>
perbaikan bug dan message
</commit_message>
<xml_diff>
--- a/input/contoh_excel.xlsx
+++ b/input/contoh_excel.xlsx
@@ -593,7 +593,7 @@
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr">
         <is>
-          <t>gagal - HTTP 429</t>
+          <t>gagal - Usaha ini sudah diground check oleh user lain. Terima kasih!</t>
         </is>
       </c>
     </row>
@@ -15881,7 +15881,7 @@
       <c r="H396" t="inlineStr"/>
       <c r="I396" t="inlineStr">
         <is>
-          <t>gagal - HTTP 429</t>
+          <t>gagal</t>
         </is>
       </c>
     </row>

</xml_diff>